<commit_message>
feat(product selection): done fully
</commit_message>
<xml_diff>
--- a/storage/app/private/excel/export-templates/product-selection.xlsx
+++ b/storage/app/private/excel/export-templates/product-selection.xlsx
@@ -16,10 +16,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1765362961" val="1228" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1765362961" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1765362961" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1765362961"/>
+      <pm:revision xmlns:pm="smNativeData" day="1765430351" val="1228" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1765430351" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1765430351" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1765430351"/>
     </ext>
   </extLst>
 </workbook>
@@ -253,7 +253,7 @@
     <numFmt numFmtId="3" formatCode="#,##0"/>
     <numFmt numFmtId="2" formatCode="0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,7 +261,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -276,7 +276,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -291,7 +291,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="240" lang="default"/>
             <pm:ea face="SimSun" sz="240" lang="default"/>
@@ -307,7 +307,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" fgClr="7030A0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" fgClr="7030A0" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -323,7 +323,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -339,7 +339,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -355,26 +355,10 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="240" lang="default" i="1"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <b/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" fgClr="FFFFFF" ulstyle="none" kern="1">
-            <pm:latin face="Calibri Light" sz="180" lang="default" weight="bold"/>
-            <pm:cs face="Times New Roman" sz="180" lang="default" weight="bold"/>
-            <pm:ea face="SimSun" sz="180" lang="default" weight="bold"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -387,7 +371,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765362961" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="180" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="180" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="180" lang="default" weight="bold"/>
@@ -396,7 +380,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,7 +396,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -423,7 +407,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -434,7 +418,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -445,7 +429,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -456,7 +440,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -467,7 +451,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="0092D050" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -478,7 +462,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00008000" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00008000" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -489,7 +473,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -500,7 +484,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -511,68 +495,13 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF660066"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF660066"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00D1D1"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="82" fgClr="0000FFFF" bgLvl="18" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00D1D1"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="82" fgClr="0000FFFF" bgLvl="18" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="12">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -588,7 +517,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
+          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
         </ext>
       </extLst>
     </border>
@@ -607,7 +536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -631,7 +560,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -655,7 +584,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -679,7 +608,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -703,7 +632,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -727,7 +656,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
+          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
         </ext>
       </extLst>
     </border>
@@ -746,7 +675,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
+          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
         </ext>
       </extLst>
     </border>
@@ -765,7 +694,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -789,7 +718,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -813,7 +742,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -837,112 +766,12 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
+          <pm:border xmlns:pm="smNativeData" id="1765430351">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961">
-            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765362961"/>
         </ext>
       </extLst>
     </border>
@@ -1046,7 +875,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1060,7 +889,7 @@
           <bgColor rgb="FF92D050"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -1072,7 +901,7 @@
           <bgColor rgb="FF92D050"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1765362961" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -1082,15 +911,16 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1765362961" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1765430351" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1765362961" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1765430351" count="6">
         <pm:color name="Color 24" rgb="7030A0"/>
         <pm:color name="Color 25" rgb="3366FF"/>
         <pm:color name="Color 26" rgb="660066"/>
         <pm:color name="Color 27" rgb="92D050"/>
         <pm:color name="Color 28" rgb="008000"/>
+        <pm:color name="Color 29" rgb="00D1D1"/>
       </pm:colors>
     </ext>
   </extLst>
@@ -1354,11 +1184,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:BY23"/>
+  <dimension ref="A1:BY24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.60"/>
@@ -1815,143 +1645,143 @@
       <c r="BX3" s="16"/>
       <c r="BY3" s="16"/>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-    </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19"/>
-    </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>54</v>
-      </c>
+      <c r="A9" s="20"/>
+      <c r="B9" s="19"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B13" s="23" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="23" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B24" s="23" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1975,13 +1805,13 @@
     <mergeCell ref="BT1:BV1"/>
     <mergeCell ref="BW1:BY1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L1:Z1048564">
+  <conditionalFormatting sqref="L1:Z1048565">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>1</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A23">
+  <conditionalFormatting sqref="A10:A24">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>1</formula>
       <formula>1</formula>
@@ -1990,7 +1820,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1765362961" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1765430351" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1999,16 +1829,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1765362961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1765362961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1765362961" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1765362961" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1765430351" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1765430351" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1765430351" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1765430351" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1765362961" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1765430351" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
refactor(Product selection): optimize file generation time
</commit_message>
<xml_diff>
--- a/storage/app/private/excel/export-templates/product-selection.xlsx
+++ b/storage/app/private/excel/export-templates/product-selection.xlsx
@@ -16,10 +16,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1765430351" val="1228" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1765430351" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1765430351" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1765430351"/>
+      <pm:revision xmlns:pm="smNativeData" day="1765449183" val="1228" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1765449183" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1765449183" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1765449183"/>
     </ext>
   </extLst>
 </workbook>
@@ -261,7 +261,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -276,7 +276,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -291,7 +291,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="240" lang="default"/>
             <pm:ea face="SimSun" sz="240" lang="default"/>
@@ -307,7 +307,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" fgClr="7030A0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" fgClr="7030A0" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -323,7 +323,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -339,7 +339,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="240" lang="default" weight="bold"/>
@@ -355,7 +355,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="240" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="240" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="240" lang="default" i="1"/>
@@ -371,7 +371,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1765430351" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1765449183" ulstyle="none" kern="1">
             <pm:latin face="Calibri Light" sz="180" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="180" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="180" lang="default" weight="bold"/>
@@ -396,7 +396,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -407,7 +407,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -418,7 +418,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -429,7 +429,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -440,7 +440,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -451,7 +451,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="0092D050" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -462,7 +462,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00008000" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00008000" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -473,7 +473,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="003366FF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -484,7 +484,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -495,7 +495,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="00660066" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -517,7 +517,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
+          <pm:border xmlns:pm="smNativeData" id="1765449183"/>
         </ext>
       </extLst>
     </border>
@@ -536,7 +536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -560,7 +560,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -584,7 +584,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -608,7 +608,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -632,7 +632,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -656,7 +656,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
+          <pm:border xmlns:pm="smNativeData" id="1765449183"/>
         </ext>
       </extLst>
     </border>
@@ -675,7 +675,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351"/>
+          <pm:border xmlns:pm="smNativeData" id="1765449183"/>
         </ext>
       </extLst>
     </border>
@@ -694,7 +694,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -718,7 +718,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -742,7 +742,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -766,7 +766,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1765430351">
+          <pm:border xmlns:pm="smNativeData" id="1765449183">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -889,7 +889,7 @@
           <bgColor rgb="FF92D050"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -901,7 +901,7 @@
           <bgColor rgb="FF92D050"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1765430351" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1765449183" type="1" fgLvl="100" fgClr="0092D050" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -911,10 +911,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1765430351" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1765449183" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1765430351" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1765449183" count="6">
         <pm:color name="Color 24" rgb="7030A0"/>
         <pm:color name="Color 25" rgb="3366FF"/>
         <pm:color name="Color 26" rgb="660066"/>
@@ -1184,11 +1184,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:BY24"/>
+  <dimension ref="A1:BZ24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.60"/>
@@ -1645,6 +1645,76 @@
       <c r="BX3" s="16"/>
       <c r="BY3" s="16"/>
     </row>
+    <row r="4" spans="1:78">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="BZ4"/>
+    </row>
+    <row r="5" spans="1:78">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="BZ5"/>
+    </row>
     <row r="6" spans="1:2">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
@@ -1805,7 +1875,7 @@
     <mergeCell ref="BT1:BV1"/>
     <mergeCell ref="BW1:BY1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L1:Z1048565">
+  <conditionalFormatting sqref="L1:Z3 L6:Z1048565">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>1</formula>
       <formula>1</formula>
@@ -1820,7 +1890,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1765430351" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1765449183" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1829,16 +1899,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1765430351" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1765430351" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1765430351" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1765430351" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1765449183" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1765449183" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1765449183" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1765449183" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1765430351" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1765449183" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>